<commit_message>
step 1 to 3
Get started  Add a controller  Add a view
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E5C22-FA72-4EE6-A5BF-21C9EAC52A85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5235E69-CF41-4277-840A-E58A866EE6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="1890" windowWidth="17085" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4725" yWindow="2430" windowWidth="21195" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>week1</t>
   </si>
@@ -123,21 +123,28 @@
     <t>hour 20</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Read "What is the MVC pattern?"
-2. Create new Github repo and folder 3. Install Visual Studio 2019 and .NET Core 3.1 SDK
-4. Create individul time sheet </t>
+    <t>1. Fix Source Tree credential problem(unsuccessfull)</t>
+  </si>
+  <si>
+    <t>1. Fix GitHub Desktop credential problem(unsuccessfull)</t>
   </si>
   <si>
     <t>1. Install SQL Express
 2. Install Resharper
-3. Install Source Tree
-4.</t>
-  </si>
-  <si>
-    <t>1. Fix Source Tree credential problem(unsuccessfull)</t>
-  </si>
-  <si>
-    <t>2. Fix GitHub credential problem(unsuccessfull)</t>
+3. Install Source Tree(credential problem)
+4. Install GitHub Desktop(credential problem)</t>
+  </si>
+  <si>
+    <t>1. Fix GitHub credential problem(successfull)
+2. Complete step 1 "Get started"
+3. Complete step 2 "Add a controller"
+4. Complete step 3 "Add a view"</t>
+  </si>
+  <si>
+    <t>1. Read "What is the MVC pattern?"
+2. Create new Github repo and folder 3. Install Visual Studio 2019 and .NET Core 3.1 SDK
+4. Create individul time sheet 
+5. Join the WhatsApp group</t>
   </si>
 </sst>
 </file>
@@ -153,15 +160,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,19 +194,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -216,187 +226,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>23834</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6032</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>742951</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{837D0687-7B6E-465B-BA1E-7A7677532793}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2909909" y="1238251"/>
-          <a:ext cx="3030198" cy="742950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>23834</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>933451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>6032</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>781050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14368E51-5B1A-44C8-BC87-37AA85AB82B3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2909909" y="1219201"/>
-          <a:ext cx="3030198" cy="800099"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>51948</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>238126</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>198623</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37A7A757-7139-42A5-8DF4-55487A6055BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4157223" y="2333626"/>
-          <a:ext cx="5023475" cy="809624"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1000124</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B0D1589-47B4-43A0-A05B-55FDFB746941}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3552825" y="3143251"/>
-          <a:ext cx="2466975" cy="904873"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -665,7 +494,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,159 +503,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complet step 3 and step 4
complet step 3 and step 4, update time sheet
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5235E69-CF41-4277-840A-E58A866EE6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFBB85D-3CB2-4209-83DD-CC02241940DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4725" yWindow="2430" windowWidth="21195" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>week1</t>
   </si>
@@ -135,16 +135,20 @@
 4. Install GitHub Desktop(credential problem)</t>
   </si>
   <si>
-    <t>1. Fix GitHub credential problem(successfull)
-2. Complete step 1 "Get started"
-3. Complete step 2 "Add a controller"
-4. Complete step 3 "Add a view"</t>
-  </si>
-  <si>
     <t>1. Read "What is the MVC pattern?"
 2. Create new Github repo and folder 3. Install Visual Studio 2019 and .NET Core 3.1 SDK
 4. Create individul time sheet 
 5. Join the WhatsApp group</t>
+  </si>
+  <si>
+    <t>1. Fix GitHub credential problem(successfull)
+2. Complete step 1 "Get started"
+3. Complete step 2 "Add a controller"
+4. Complete part of  step 3 "Add a view"</t>
+  </si>
+  <si>
+    <t>1. Complete step3 "Add a view"
+2. Complete step4 "Add a model"</t>
   </si>
 </sst>
 </file>
@@ -194,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -207,9 +211,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -572,19 +573,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">

</xml_diff>

<commit_message>
step 5 - 7
Work with a database
Controller actions and views
Add search
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFBB85D-3CB2-4209-83DD-CC02241940DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAB8109-92CD-4BEE-A2A2-4F8AE75B7A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="2430" windowWidth="21195" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1680" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>week1</t>
   </si>
@@ -149,6 +149,14 @@
   <si>
     <t>1. Complete step3 "Add a view"
 2. Complete step4 "Add a model"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Complete step5 "Work with a database"
+2. Complete part of step 6 "Controller actions and views" </t>
+  </si>
+  <si>
+    <t>1. Complete step 6 "Controller actions and views" 
+2. Complete step 7 "Add search"</t>
   </si>
 </sst>
 </file>
@@ -495,7 +503,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,17 +597,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">

</xml_diff>

<commit_message>
step 8 - 10
Add a new field
Add validation
Examine the Details and Delete methods
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAB8109-92CD-4BEE-A2A2-4F8AE75B7A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F06D3E-511D-4C79-AA23-8483FC5A65EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1680" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11175" yWindow="915" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>week1</t>
   </si>
@@ -157,6 +157,11 @@
   <si>
     <t>1. Complete step 6 "Controller actions and views" 
 2. Complete step 7 "Add search"</t>
+  </si>
+  <si>
+    <t>1. Complete step 8 " Add a new field"
+2. Complete step 9 " Add validation"
+3. Complete step 9 " Examine Details and Delete"</t>
   </si>
 </sst>
 </file>
@@ -502,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,11 +618,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">

</xml_diff>

<commit_message>
Week 2 task update
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4358DCD7-B5A6-4486-8895-2CDB9B2332D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B77CF02-BC26-4017-B9B0-C5A4EEDF888D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="2190" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,16 +216,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -233,11 +245,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -254,14 +282,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +677,7 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -667,7 +699,7 @@
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -676,7 +708,7 @@
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -685,7 +717,7 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -694,14 +726,14 @@
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">

</xml_diff>

<commit_message>
week 3 tasks update
week 3 tasks update
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GoogleDrive\study\2020\Semester 2\HIT 339\GitRepo\HIT339_Qingyuan_Zeng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B77CF02-BC26-4017-B9B0-C5A4EEDF888D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D0D0F-01CE-4D36-B263-59D6B2196616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1665" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>week1</t>
   </si>
@@ -189,12 +189,29 @@
     <t>1. Completing the second part of week 2 task.（Not finished）
 2. Fixing "EmailAddressAttribute" issue</t>
   </si>
+  <si>
+    <t>1. Completing admin movie task (finished)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Read "Web services vs Web-Api".
+2. Read "Ef discussion".
+3. Read "LINQ".
+4. Completing "Creating web api".
+</t>
+  </si>
+  <si>
+    <t>1. Completing "Creating javascript app using the api's".
+2. Read "swagger"</t>
+  </si>
+  <si>
+    <t>1. Whatching video and learning how to make documentation using 'Swagger'(unfinished)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,8 +240,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +259,14 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,12 +289,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -279,16 +317,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,13 +622,14 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,6 +680,9 @@
       <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="D2" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -641,7 +692,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -651,6 +702,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="6"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -660,6 +712,9 @@
         <v>41</v>
       </c>
       <c r="C5" s="6"/>
+      <c r="D5" s="9" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -669,6 +724,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="6"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -677,9 +733,10 @@
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -691,6 +748,9 @@
       <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="D8" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -699,7 +759,10 @@
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -708,7 +771,8 @@
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -717,7 +781,7 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -726,14 +790,14 @@
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="8"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -784,9 +848,12 @@
       <c r="B21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to identity features
create registeration form with fields validation
create login page
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E23A27E-6E65-4569-AD64-A2CED066DD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C2DB42-3E2E-4A98-803B-871749DD6CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="2250" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="975" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>week1</t>
   </si>
@@ -245,6 +245,9 @@
 2. Building environment for Angular
 3. Read materials about Angular
 4. Complete task 2 in week 4</t>
+  </si>
+  <si>
+    <t>1. Create item</t>
   </si>
 </sst>
 </file>
@@ -673,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,6 +867,9 @@
       <c r="D12" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="E12" s="10" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -874,6 +880,7 @@
       <c r="D13" s="6" t="s">
         <v>53</v>
       </c>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -883,6 +890,7 @@
       <c r="D14" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -890,45 +898,49 @@
       </c>
       <c r="B15" s="1"/>
       <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C2:C6"/>
@@ -937,6 +949,7 @@
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E6:E11"/>
+    <mergeCell ref="E12:E18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
organize the e shop project
Organize the project, removing identity features and other unnecessary code that were auto-generated by visual studio 2019
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C2DB42-3E2E-4A98-803B-871749DD6CD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B715FE3-2AD6-485F-BBBE-31968D67A601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="975" windowWidth="21945" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11700" yWindow="150" windowWidth="16770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>week1</t>
   </si>
@@ -247,7 +247,48 @@
 4. Complete task 2 in week 4</t>
   </si>
   <si>
-    <t>1. Create item</t>
+    <t>hour 21</t>
+  </si>
+  <si>
+    <t>hour 22</t>
+  </si>
+  <si>
+    <t>hour 23</t>
+  </si>
+  <si>
+    <t>hour 24</t>
+  </si>
+  <si>
+    <t>hour 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Create assignment 1 project using Angular
+2. Install Visual Studio Code and useful extentions
+3. Create component for a item card 
+4. Create component for item list 
+5. Add css to item card using bootstrap
+6. create service to make HTTP calls to retrieve data for each item card
+7. Modify HTTP data using Pipe
+8. Create routes for items in the navigation menu
+9. Create new component for displaying details of each item
+10. create next page button using event binding
+11. Apply routing features to display different list of items based on different page urls
+12. Apply defult picture for items with no image property
+13. Create a new component for adding new items
+14. Create a form for the new component using template driven approach
+15. Apply validations to the form
+16. Create animations and error notifacations that will display when inputs is not valid
+17. Create a new component for user registration
+18. Create a form for the new component using reactive form approach
+19. apply validations
+20. Create animations and error notifacations that will display when inputs is not valid using alertify
+21. Organize the code for the form using 'FormBuilder'
+22. Create a new service for adding new account information from the registration form to the local storage
+</t>
+  </si>
+  <si>
+    <t>1. Organize the project, removing identity features and other unnecessary code that were auto-generated by visual studio 2019
+2. Fix bootstrap problem and other startup issues after the operation</t>
   </si>
 </sst>
 </file>
@@ -346,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -392,6 +433,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -674,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E18"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +732,7 @@
     <col min="5" max="5" width="31.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -726,7 +770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -743,7 +787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -754,7 +798,7 @@
       <c r="D3" s="13"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -765,7 +809,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -778,7 +822,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -791,7 +835,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -804,7 +848,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -819,7 +863,7 @@
       </c>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -832,7 +876,7 @@
       </c>
       <c r="E9" s="15"/>
     </row>
-    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -843,7 +887,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -856,7 +900,7 @@
       </c>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -867,11 +911,11 @@
       <c r="D12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="E12" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -880,9 +924,9 @@
       <c r="D13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -890,57 +934,93 @@
       <c r="D14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="E25:E26"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C2:C6"/>
@@ -949,7 +1029,7 @@
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E6:E11"/>
-    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="E12:E24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
login, logout and dropdown menu
update login, logout functionalities and create dropdown menu
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B715FE3-2AD6-485F-BBBE-31968D67A601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A46CD8F-8A56-437C-92E7-94FA878FB8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="150" windowWidth="16770" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4725" yWindow="15" windowWidth="20850" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>week1</t>
   </si>
@@ -196,9 +196,6 @@
   <si>
     <t>1. Completing the second part of week 2 task.（Not finished）
 2. Fixing "EmailAddressAttribute" issue</t>
-  </si>
-  <si>
-    <t>1. Completing admin movie task (finished)</t>
   </si>
   <si>
     <t xml:space="preserve">1. Read "Web services vs Web-Api".
@@ -288,7 +285,20 @@
   </si>
   <si>
     <t>1. Organize the project, removing identity features and other unnecessary code that were auto-generated by visual studio 2019
+2. Fix .git problem
 2. Fix bootstrap problem and other startup issues after the operation</t>
+  </si>
+  <si>
+    <t>1. Completing admin movie task (finished)+A2:D7B2:D7C2:D7D2D2:E11D2:F11</t>
+  </si>
+  <si>
+    <t>1. Create login and logout functionalities
+2. create login component
+3. Create authentication service
+4. Apply token to track the loggin status 
+5. Apply dynamic changing status to the navagation menu
+6. Install Ngx-bootstrap
+7. Add a dropdown menu to display the user profile section at the navigation bar</t>
   </si>
 </sst>
 </file>
@@ -387,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -417,6 +427,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -435,7 +448,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -720,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +743,7 @@
     <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,14 +791,17 @@
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>55</v>
+      <c r="D2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,9 +811,10 @@
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -805,9 +823,10 @@
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="17"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -816,11 +835,11 @@
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -829,10 +848,10 @@
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15" t="s">
-        <v>54</v>
+      <c r="C6" s="12"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,8 +864,8 @@
       <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -855,13 +874,13 @@
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="15"/>
+        <v>47</v>
+      </c>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -870,11 +889,11 @@
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="15"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -883,9 +902,9 @@
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -894,11 +913,11 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="15"/>
+        <v>49</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -907,12 +926,12 @@
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -920,106 +939,107 @@
         <v>23</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="16"/>
+        <v>52</v>
+      </c>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="D14" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="16"/>
+      <c r="D14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="16"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="E16" s="16"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="E17" s="16"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="E18" s="16"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="E19" s="16"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="E20" s="16"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="E21" s="16"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="16"/>
+        <v>59</v>
+      </c>
+      <c r="E26" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="F2:F4"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="D14:D15"/>

</xml_diff>

<commit_message>
1. Update CRUD functionality to identity and items
1. Update CRUD functionality to identity and items
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A46CD8F-8A56-437C-92E7-94FA878FB8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217A45B-152D-4633-AA81-78E03FBC160E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4725" yWindow="15" windowWidth="20850" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="855" windowWidth="21270" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>week1</t>
   </si>
@@ -299,6 +299,21 @@
 5. Apply dynamic changing status to the navagation menu
 6. Install Ngx-bootstrap
 7. Add a dropdown menu to display the user profile section at the navigation bar</t>
+  </si>
+  <si>
+    <t>1. Combine Angular project with Entity Framwork</t>
+  </si>
+  <si>
+    <t>1. Improve add item page and connect it with local database using entity framwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Update item detail component </t>
+  </si>
+  <si>
+    <t>1. Add user profile where user information can be modified</t>
+  </si>
+  <si>
+    <t>1. Update CRUD functionality to identity and items</t>
   </si>
 </sst>
 </file>
@@ -397,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -427,7 +442,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -449,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -733,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +762,7 @@
     <col min="4" max="4" width="39.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -762,7 +781,7 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -802,6 +821,9 @@
       </c>
       <c r="F2" s="11" t="s">
         <v>63</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -815,6 +837,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="11"/>
       <c r="F3" s="17"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -827,6 +850,9 @@
       <c r="D4" s="14"/>
       <c r="E4" s="11"/>
       <c r="F4" s="17"/>
+      <c r="G4" s="16" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -840,6 +866,7 @@
         <v>46</v>
       </c>
       <c r="E5" s="11"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -853,6 +880,7 @@
       <c r="E6" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -866,6 +894,7 @@
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -881,6 +910,9 @@
         <v>47</v>
       </c>
       <c r="E8" s="16"/>
+      <c r="G8" s="16" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -894,6 +926,7 @@
         <v>48</v>
       </c>
       <c r="E9" s="16"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -905,6 +938,9 @@
       <c r="C10" s="13"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
+      <c r="G10" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -918,6 +954,9 @@
         <v>49</v>
       </c>
       <c r="E11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -930,9 +969,10 @@
       <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="18" t="s">
         <v>60</v>
       </c>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -943,7 +983,8 @@
       <c r="D13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -953,7 +994,8 @@
       <c r="D14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="18"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -961,73 +1003,74 @@
       </c>
       <c r="B15" s="1"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="18"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="18" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1035,21 +1078,25 @@
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="E26" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G7"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="E12:E24"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G11:G15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="C8:C13"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="E12:E24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
backup before adding shopping cart
</commit_message>
<xml_diff>
--- a/Individual Timesheet.xlsx
+++ b/Individual Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GitHub\HIT339_Qingyuan_Zeng\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217A45B-152D-4633-AA81-78E03FBC160E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B94D945-A52C-42CB-B5EC-9A31EE8B657A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="855" windowWidth="21270" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -458,15 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -752,7 +752,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,6 +763,7 @@
     <col min="5" max="5" width="31.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
     <col min="7" max="7" width="32.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -810,19 +811,19 @@
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -833,11 +834,11 @@
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -846,11 +847,11 @@
       <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -861,12 +862,12 @@
       <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="12"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -875,12 +876,12 @@
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -892,9 +893,9 @@
       <c r="C7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -903,14 +904,14 @@
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -921,12 +922,12 @@
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="E9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -935,9 +936,9 @@
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="11"/>
       <c r="G10" s="10" t="s">
         <v>67</v>
       </c>
@@ -949,12 +950,12 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="G11" s="16" t="s">
+      <c r="E11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -965,112 +966,112 @@
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="13"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="G13" s="16"/>
+      <c r="E13" s="14"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="G14" s="16"/>
+      <c r="E14" s="14"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="18"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="14"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="14"/>
     </row>
     <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="E18" s="18"/>
+      <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="14"/>
     </row>
     <row r="22" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1078,10 +1079,16 @@
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="F2:F4"/>
@@ -1091,12 +1098,6 @@
     <mergeCell ref="E12:E24"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G11:G15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>